<commit_message>
Edit post, user entity(seller, buyers 구분)
</commit_message>
<xml_diff>
--- a/CucumberMarket_ResolverPlan.xlsx
+++ b/CucumberMarket_ResolverPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimyh\Desktop\GitHub\cucumber-market-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8B779D-94D3-4CEC-9176-79FB4150106F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F09200-7DF1-40F9-9751-45A0D022A19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-144" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BC42B4B1-B66D-4EFB-8274-F6B84C45D884}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{BC42B4B1-B66D-4EFB-8274-F6B84C45D884}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -165,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>getLikedPostList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>getChatList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -298,6 +294,10 @@
   </si>
   <si>
     <t>getUserProfile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getLikedPosts</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2754,7 +2754,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2810,7 +2810,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -2824,7 +2824,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>25</v>
@@ -2890,7 +2890,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>11</v>
@@ -2914,8 +2914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9F4F75-3170-44E2-9B3A-E2D927C5BCE7}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2964,16 +2964,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2984,7 +2984,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>24</v>
@@ -2993,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3107,7 +3107,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3156,7 +3156,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
@@ -3165,7 +3165,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3247,8 +3247,9 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3257,8 +3258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19302ED-4C72-4653-9698-E02F0B2AF247}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3307,16 +3308,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3327,16 +3328,16 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3347,7 +3348,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>24</v>
@@ -3367,13 +3368,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>11</v>
@@ -3410,7 +3411,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3423,7 +3424,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3459,13 +3460,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>
@@ -3502,7 +3503,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3515,7 +3516,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3551,13 +3552,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>
@@ -3571,13 +3572,13 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>11</v>
@@ -3591,13 +3592,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>11</v>
@@ -3689,7 +3690,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Refactory like resolvers & service
</commit_message>
<xml_diff>
--- a/CucumberMarket_ResolverPlan.xlsx
+++ b/CucumberMarket_ResolverPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimyh\Desktop\GitHub\cucumber-market-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F09200-7DF1-40F9-9751-45A0D022A19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F6CD9C-7BAF-463E-A28E-FB014515B534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{BC42B4B1-B66D-4EFB-8274-F6B84C45D884}"/>
+    <workbookView xWindow="22932" yWindow="-144" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BC42B4B1-B66D-4EFB-8274-F6B84C45D884}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
   <si>
     <t>구분</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,14 +222,6 @@
   </si>
   <si>
     <t>getPostDetail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>createChatRoom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>exitChatRoom</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -270,10 +262,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>enterChatRoom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>dateTime, chatId</t>
   </si>
   <si>
@@ -298,6 +286,18 @@
   </si>
   <si>
     <t>getLikedPosts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getChatRoomInList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getChatRoomInPost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>postId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2395,8 +2395,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4EA047C8-1AE1-4415-B6AF-DD24A9FFF284}" name="표2_81214" displayName="표2_81214" ref="A2:F6" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
-  <autoFilter ref="A2:F6" xr:uid="{0F308771-8971-4D80-AD93-1DC3E5B4D66F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4EA047C8-1AE1-4415-B6AF-DD24A9FFF284}" name="표2_81214" displayName="표2_81214" ref="A2:F5" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+  <autoFilter ref="A2:F5" xr:uid="{0F308771-8971-4D80-AD93-1DC3E5B4D66F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BBCBE50F-D321-4FC7-8FC4-119E7664A75D}" name="구분" dataDxfId="38"/>
     <tableColumn id="2" xr3:uid="{156CC640-9210-4F51-8554-9F4E5514AB0C}" name="Type" dataDxfId="37"/>
@@ -2810,7 +2810,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -2824,7 +2824,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>25</v>
@@ -2890,7 +2890,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>11</v>
@@ -2970,7 +2970,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>38</v>
@@ -2993,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3156,7 +3156,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
@@ -3256,10 +3256,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19302ED-4C72-4653-9698-E02F0B2AF247}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3314,85 +3314,61 @@
         <v>46</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
+      <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>61</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="O12" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="O14" s="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O11" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3400,8 +3376,9 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3552,13 +3529,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>
@@ -3572,13 +3549,13 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>11</v>
@@ -3690,7 +3667,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>

</xml_diff>